<commit_message>
1. Lengthen Y/N screens by 2 seconds, from 5 to 7 seconds 2. The white borders for each task seem to be alternating between 5 and 10 seconds, can we make them all 10 seconds? 3. Change the instructions for each task
</commit_message>
<xml_diff>
--- a/instructions.xlsx
+++ b/instructions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacquessinger/Documents/Academics/Research/BCI Projects/MIL_PsychoPy_fMRI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C861AB6D-0A45-6D42-8E6C-A9934884C84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72009ADC-6A70-7B43-80D4-A16FC5365EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39420" yWindow="4440" windowWidth="27640" windowHeight="15660" xr2:uid="{9A7238A4-5910-8C4D-A178-E03BBFDD2D76}"/>
+    <workbookView xWindow="3260" yWindow="1460" windowWidth="27640" windowHeight="15660" xr2:uid="{9A7238A4-5910-8C4D-A178-E03BBFDD2D76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,16 +50,36 @@
     <t>AI_instructions</t>
   </si>
   <si>
-    <t>In this task, you will read scenarios describing how your life purpose is disrupted by AI.\n \n • When the text box has a white border, simply read the scenario as it appears. \n \n • When the text box has a &lt;c=#008000&gt;green&lt;/c&gt; border, read the scenario carefully, reflect on how this integration disrupts your purpose, and try to reframe it. \n \n  • When the text box has a &lt;c=#FF0000&gt;red&lt;/c&gt; border, count the number vowels, and continue this counting task until the next screen appears.</t>
-  </si>
-  <si>
-    <t>In this task, you will read some of your personal statements. \n \n • When the text box has a white border, simply read the text. \n \n • When the text box has a &lt;c=#008000&gt;green&lt;/c&gt; border, think about all the ways you are significant to this person. Bring to mind specific actions or moments where your presence mattered. \n \n • When the text box has a &lt;c=#FF0000&gt;red&lt;/c&gt; border, count how many vowels appear. Keep repeating this counting task until the next screen appears. \n \n Press any key when you’re ready!</t>
-  </si>
-  <si>
-    <t>In this task, you will read a short phrases describing some of your life purposes. \n \n • When the text box has a white border, simply read the sentence as it appears. \n \n • When the text box has a &lt;c=#008000&gt;green&lt;/c&gt; border, reflect on the life purpose shown and consider how you might work toward it. \n \n • When the text box has a &lt;c=#FF0000&gt;red&lt;/c&gt; border, count the number of vowels and continue this counting task until the next screen appears. \n \nPress any button when you're ready.</t>
-  </si>
-  <si>
-    <t>In this task, you’ll see short phrases describing  events from your life.\n \n • When the text has a white border, simply read the text \n \n • When the text box has a &lt;c=#008000&gt;green&lt;/c&gt; border, think about how these events fit together and form a coherent life story. \n \n • When the text box has a &lt;c=#FF0000&gt;red&lt;/c&gt; border, count the number of vowels. Keep repeating this counting task until the next screen appears. \n \n Press any key when you’re ready!</t>
+    <t>In this task, you will read scenarios describing disruptions to your life’s purpose.
+Try to imagine these as realistically as you can.
+• &lt;c=white&gt;White&lt;/c&gt; border: read the sentence.
+• &lt;c=#008000&gt;Green&lt;/c&gt; border: read the scenario and try to reframe a new purpose despite the disruption.
+• &lt;c=#FF0000&gt;Red&lt;/c&gt; border: count the number of vowels and keep doing so until the next screen appears.
+Press any key when you're ready.</t>
+  </si>
+  <si>
+    <t>In this task, you’ll see phrases about events in your life.
+When the text box has a:
+• &lt;c=white&gt;White&lt;/c&gt; border: read the sentence.
+• &lt;c=#008000&gt;Green&lt;/c&gt; border: reflect on how these events fit together to form your life story.
+• &lt;c=#FF0000&gt;Red&lt;/c&gt; border: count the number of vowels and keep doing so until the next screen appears.
+Press any key when you're ready.</t>
+  </si>
+  <si>
+    <t>In this task, you will read some of your personal statements.
+When the text box has a:
+• &lt;c=white&gt;White&lt;/c&gt; border: read the sentence.
+• &lt;c=#008000&gt;Green&lt;/c&gt; border: think about the ways you are significant to this person or entity. Bring to mind specific moments where your presence mattered.
+• &lt;c=#FF0000&gt;Red&lt;/c&gt; border: count the number of vowels and keep doing so until the next screen appears.
+Press any key when you’re ready.</t>
+  </si>
+  <si>
+    <t>In this task, you will read phrases about your life purposes.
+When the text box has a:
+• &lt;c=white&gt;White&lt;/c&gt; border: read the sentence.
+• &lt;c=#008000&gt;Green&lt;/c&gt; border: reflect on that life purpose and how you can work toward it.
+• &lt;c=#FF0000&gt;Red&lt;/c&gt; border: count the number of vowels and keep doing so until the next screen appears.
+Press any button when you’re ready.</t>
   </si>
 </sst>
 </file>
@@ -442,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{739FF048-AB0F-3040-86E5-A0FF536BD22B}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -473,13 +493,13 @@
     </row>
     <row r="2" spans="1:4" ht="161" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>4</v>

</xml_diff>